<commit_message>
çeşitli değişiklikler ve eklemeler yapıldı
</commit_message>
<xml_diff>
--- a/ders1.xlsx
+++ b/ders1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efsan\Desktop\sınav otomasyon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efsan\Documents\GitHub\exam-automation-01-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A655B05A-F0C6-413C-8AB0-E5992933F72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453DB701-029C-440A-B8AC-B90A9B16D300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>ahmet</t>
   </si>
@@ -36,10 +36,13 @@
     <t>ali</t>
   </si>
   <si>
-    <t>veli</t>
-  </si>
-  <si>
     <t>İsim</t>
+  </si>
+  <si>
+    <t>Numara</t>
+  </si>
+  <si>
+    <t>fatma</t>
   </si>
 </sst>
 </file>
@@ -357,37 +360,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>201008</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>201009</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>201010</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>201011</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>